<commit_message>
Add back Shunt data.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_shuntsw.xlsx
+++ b/andes/cases/ieee14/ieee14_shuntsw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F896555-A1C1-3144-968B-F8EB7B996756}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1486F9FE-A6F5-AA46-BAED-494C32590EB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,22 +18,23 @@
     <sheet name="PQ" sheetId="3" r:id="rId3"/>
     <sheet name="PV" sheetId="4" r:id="rId4"/>
     <sheet name="Slack" sheetId="5" r:id="rId5"/>
-    <sheet name="ShuntSw" sheetId="15" r:id="rId6"/>
-    <sheet name="Line" sheetId="7" r:id="rId7"/>
-    <sheet name="Area" sheetId="8" r:id="rId8"/>
-    <sheet name="GENROU" sheetId="9" r:id="rId9"/>
-    <sheet name="TGOV1" sheetId="10" r:id="rId10"/>
-    <sheet name="EXST1" sheetId="11" r:id="rId11"/>
-    <sheet name="ESST3A" sheetId="12" r:id="rId12"/>
-    <sheet name="BusFreq" sheetId="13" r:id="rId13"/>
-    <sheet name="ACEc" sheetId="14" r:id="rId14"/>
+    <sheet name="Shunt" sheetId="16" r:id="rId6"/>
+    <sheet name="ShuntSw" sheetId="15" r:id="rId7"/>
+    <sheet name="Line" sheetId="7" r:id="rId8"/>
+    <sheet name="Area" sheetId="8" r:id="rId9"/>
+    <sheet name="GENROU" sheetId="9" r:id="rId10"/>
+    <sheet name="TGOV1" sheetId="10" r:id="rId11"/>
+    <sheet name="EXST1" sheetId="11" r:id="rId12"/>
+    <sheet name="ESST3A" sheetId="12" r:id="rId13"/>
+    <sheet name="BusFreq" sheetId="13" r:id="rId14"/>
+    <sheet name="ACEc" sheetId="14" r:id="rId15"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="182">
   <si>
     <t>uid</t>
   </si>
@@ -573,13 +574,19 @@
   </si>
   <si>
     <t>dt</t>
+  </si>
+  <si>
+    <t>Shunt_1</t>
+  </si>
+  <si>
+    <t>Shunt_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,6 +615,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -658,7 +673,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -671,6 +686,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1058,6 +1076,523 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:AB6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>69</v>
+      </c>
+      <c r="J2">
+        <v>60</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0.15</v>
+      </c>
+      <c r="O2">
+        <v>0.6</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0.09</v>
+      </c>
+      <c r="S2">
+        <v>0.38</v>
+      </c>
+      <c r="T2">
+        <v>1.8</v>
+      </c>
+      <c r="U2">
+        <v>1.75</v>
+      </c>
+      <c r="V2">
+        <v>0.23</v>
+      </c>
+      <c r="W2">
+        <v>0.8</v>
+      </c>
+      <c r="X2">
+        <v>0.23</v>
+      </c>
+      <c r="Y2">
+        <v>6.5</v>
+      </c>
+      <c r="Z2">
+        <v>0.06</v>
+      </c>
+      <c r="AA2">
+        <v>0.2</v>
+      </c>
+      <c r="AB2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3">
+        <v>69</v>
+      </c>
+      <c r="J3">
+        <v>60</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>13</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0.15</v>
+      </c>
+      <c r="O3">
+        <v>0.6</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0.09</v>
+      </c>
+      <c r="S3">
+        <v>0.38</v>
+      </c>
+      <c r="T3">
+        <v>1.8</v>
+      </c>
+      <c r="U3">
+        <v>1.75</v>
+      </c>
+      <c r="V3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="W3">
+        <v>0.8</v>
+      </c>
+      <c r="X3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Y3">
+        <v>6.5</v>
+      </c>
+      <c r="Z3">
+        <v>0.06</v>
+      </c>
+      <c r="AA3">
+        <v>0.2</v>
+      </c>
+      <c r="AB3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4">
+        <v>69</v>
+      </c>
+      <c r="J4">
+        <v>60</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0.15</v>
+      </c>
+      <c r="O4">
+        <v>0.6</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0.09</v>
+      </c>
+      <c r="S4">
+        <v>0.38</v>
+      </c>
+      <c r="T4">
+        <v>1.8</v>
+      </c>
+      <c r="U4">
+        <v>1.75</v>
+      </c>
+      <c r="V4">
+        <v>0.34</v>
+      </c>
+      <c r="W4">
+        <v>0.8</v>
+      </c>
+      <c r="X4">
+        <v>0.34</v>
+      </c>
+      <c r="Y4">
+        <v>6.5</v>
+      </c>
+      <c r="Z4">
+        <v>0.06</v>
+      </c>
+      <c r="AA4">
+        <v>0.2</v>
+      </c>
+      <c r="AB4">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5">
+        <v>138</v>
+      </c>
+      <c r="J5">
+        <v>60</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0.15</v>
+      </c>
+      <c r="O5">
+        <v>0.6</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0.09</v>
+      </c>
+      <c r="S5">
+        <v>0.38</v>
+      </c>
+      <c r="T5">
+        <v>1.8</v>
+      </c>
+      <c r="U5">
+        <v>1.75</v>
+      </c>
+      <c r="V5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="W5">
+        <v>0.8</v>
+      </c>
+      <c r="X5">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Y5">
+        <v>6.5</v>
+      </c>
+      <c r="Z5">
+        <v>0.06</v>
+      </c>
+      <c r="AA5">
+        <v>0.2</v>
+      </c>
+      <c r="AB5">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6">
+        <v>69</v>
+      </c>
+      <c r="J6">
+        <v>60</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0.15</v>
+      </c>
+      <c r="O6">
+        <v>0.6</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0.09</v>
+      </c>
+      <c r="S6">
+        <v>0.38</v>
+      </c>
+      <c r="T6">
+        <v>1.8</v>
+      </c>
+      <c r="U6">
+        <v>1.75</v>
+      </c>
+      <c r="V6">
+        <v>0.34</v>
+      </c>
+      <c r="W6">
+        <v>0.8</v>
+      </c>
+      <c r="X6">
+        <v>0.34</v>
+      </c>
+      <c r="Y6">
+        <v>6.5</v>
+      </c>
+      <c r="Z6">
+        <v>0.06</v>
+      </c>
+      <c r="AA6">
+        <v>0.2</v>
+      </c>
+      <c r="AB6">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
@@ -1322,7 +1857,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -1444,7 +1979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
@@ -1860,7 +2395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -1980,7 +2515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4239113-628F-774A-BBB2-DE2B24367532}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -3594,10 +4129,122 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF7C6A67-09F9-144F-A76D-C1DEFC0D9C4F}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>138</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0.19</v>
+      </c>
+      <c r="J2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>138</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0.15</v>
+      </c>
+      <c r="J3">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD6D781A-1D81-D34A-BEBC-48956C84C41A}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
     </sheetView>
@@ -3759,7 +4406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:X21"/>
   <sheetViews>
@@ -5149,7 +5796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -5205,521 +5852,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AB6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>100</v>
-      </c>
-      <c r="I2">
-        <v>69</v>
-      </c>
-      <c r="J2">
-        <v>60</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>8</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0.15</v>
-      </c>
-      <c r="O2">
-        <v>0.6</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0.09</v>
-      </c>
-      <c r="S2">
-        <v>0.38</v>
-      </c>
-      <c r="T2">
-        <v>1.8</v>
-      </c>
-      <c r="U2">
-        <v>1.75</v>
-      </c>
-      <c r="V2">
-        <v>0.23</v>
-      </c>
-      <c r="W2">
-        <v>0.8</v>
-      </c>
-      <c r="X2">
-        <v>0.23</v>
-      </c>
-      <c r="Y2">
-        <v>6.5</v>
-      </c>
-      <c r="Z2">
-        <v>0.06</v>
-      </c>
-      <c r="AA2">
-        <v>0.2</v>
-      </c>
-      <c r="AB2">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>100</v>
-      </c>
-      <c r="I3">
-        <v>69</v>
-      </c>
-      <c r="J3">
-        <v>60</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>13</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0.15</v>
-      </c>
-      <c r="O3">
-        <v>0.6</v>
-      </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0.09</v>
-      </c>
-      <c r="S3">
-        <v>0.38</v>
-      </c>
-      <c r="T3">
-        <v>1.8</v>
-      </c>
-      <c r="U3">
-        <v>1.75</v>
-      </c>
-      <c r="V3">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="W3">
-        <v>0.8</v>
-      </c>
-      <c r="X3">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="Y3">
-        <v>6.5</v>
-      </c>
-      <c r="Z3">
-        <v>0.06</v>
-      </c>
-      <c r="AA3">
-        <v>0.2</v>
-      </c>
-      <c r="AB3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>100</v>
-      </c>
-      <c r="I4">
-        <v>69</v>
-      </c>
-      <c r="J4">
-        <v>60</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>10</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>0.15</v>
-      </c>
-      <c r="O4">
-        <v>0.6</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0.09</v>
-      </c>
-      <c r="S4">
-        <v>0.38</v>
-      </c>
-      <c r="T4">
-        <v>1.8</v>
-      </c>
-      <c r="U4">
-        <v>1.75</v>
-      </c>
-      <c r="V4">
-        <v>0.34</v>
-      </c>
-      <c r="W4">
-        <v>0.8</v>
-      </c>
-      <c r="X4">
-        <v>0.34</v>
-      </c>
-      <c r="Y4">
-        <v>6.5</v>
-      </c>
-      <c r="Z4">
-        <v>0.06</v>
-      </c>
-      <c r="AA4">
-        <v>0.2</v>
-      </c>
-      <c r="AB4">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5">
-        <v>6</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="H5">
-        <v>100</v>
-      </c>
-      <c r="I5">
-        <v>138</v>
-      </c>
-      <c r="J5">
-        <v>60</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>10</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0.15</v>
-      </c>
-      <c r="O5">
-        <v>0.6</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0.09</v>
-      </c>
-      <c r="S5">
-        <v>0.38</v>
-      </c>
-      <c r="T5">
-        <v>1.8</v>
-      </c>
-      <c r="U5">
-        <v>1.75</v>
-      </c>
-      <c r="V5">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="W5">
-        <v>0.8</v>
-      </c>
-      <c r="X5">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="Y5">
-        <v>6.5</v>
-      </c>
-      <c r="Z5">
-        <v>0.06</v>
-      </c>
-      <c r="AA5">
-        <v>0.2</v>
-      </c>
-      <c r="AB5">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6">
-        <v>8</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="H6">
-        <v>100</v>
-      </c>
-      <c r="I6">
-        <v>69</v>
-      </c>
-      <c r="J6">
-        <v>60</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>10</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6">
-        <v>0.15</v>
-      </c>
-      <c r="O6">
-        <v>0.6</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6">
-        <v>0.09</v>
-      </c>
-      <c r="S6">
-        <v>0.38</v>
-      </c>
-      <c r="T6">
-        <v>1.8</v>
-      </c>
-      <c r="U6">
-        <v>1.75</v>
-      </c>
-      <c r="V6">
-        <v>0.34</v>
-      </c>
-      <c r="W6">
-        <v>0.8</v>
-      </c>
-      <c r="X6">
-        <v>0.34</v>
-      </c>
-      <c r="Y6">
-        <v>6.5</v>
-      </c>
-      <c r="Z6">
-        <v>0.06</v>
-      </c>
-      <c r="AA6">
-        <v>0.2</v>
-      </c>
-      <c r="AB6">
-        <v>0.05</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>